<commit_message>
fix to use iep and one sample class
</commit_message>
<xml_diff>
--- a/sorting/src/test/resources/sampleClassToArrange.xlsx
+++ b/sorting/src/test/resources/sampleClassToArrange.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arutf\Documents\classOrganization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arutf\Documents\classOrganization\sorting\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9037A8-9331-4B39-A729-C13FCB899E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3107FF-173E-4CDF-9C22-2AD15003684F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{75A70F23-6CEA-406E-B64B-2FD3293A5F8B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{75A70F23-6CEA-406E-B64B-2FD3293A5F8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Teachers</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Can't have student</t>
   </si>
   <si>
-    <t>504 plan</t>
-  </si>
-  <si>
     <t>Is female</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>IEP</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B20" sqref="A1:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -498,7 +498,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -506,7 +506,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -521,23 +521,23 @@
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -545,10 +545,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -556,10 +556,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
@@ -567,28 +567,28 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -596,53 +596,53 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
         <v>28</v>
-      </c>
-      <c r="F17" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17">
-        <v>504</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" t="s">
         <v>28</v>
-      </c>
-      <c r="G18">
-        <v>504</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -650,7 +650,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>